<commit_message>
Added temporary Test Cases.xlsx file
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -5,29 +5,35 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhonebookApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79C71AC-DF10-4B89-8CB3-7D85BF5822CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24D293F-596F-48ED-9E0E-DDA8E820CE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Add a phone number" sheetId="7" r:id="rId1"/>
-    <sheet name="FundTransfer" sheetId="3" state="hidden" r:id="rId2"/>
-    <sheet name="BalenceEnquiry" sheetId="4" state="hidden" r:id="rId3"/>
-    <sheet name="Inter Bank Fund  Transfer" sheetId="5" state="hidden" r:id="rId4"/>
-    <sheet name="Change  password" sheetId="6" state="hidden" r:id="rId5"/>
+    <sheet name="2. Update a phone number" sheetId="8" r:id="rId2"/>
+    <sheet name="3. Delete a phone number" sheetId="9" r:id="rId3"/>
+    <sheet name="4. Search for a phone number by" sheetId="10" r:id="rId4"/>
+    <sheet name="FundTransfer" sheetId="3" state="hidden" r:id="rId5"/>
+    <sheet name="BalenceEnquiry" sheetId="4" state="hidden" r:id="rId6"/>
+    <sheet name="Inter Bank Fund  Transfer" sheetId="5" state="hidden" r:id="rId7"/>
+    <sheet name="Change  password" sheetId="6" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Add a phone number'!$A$1:$J$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Add a phone number'!$A$1:$J$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2. Update a phone number'!$A$1:$J$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'3. Delete a phone number'!$A$1:$J$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'4. Search for a phone number by'!$A$1:$J$84</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="213">
   <si>
     <t>TestCase#</t>
   </si>
@@ -539,6 +545,226 @@
 Name: Abdelrahman Abodief
 Email: abodief@exmail.com
 Email: mohamed@exmail.com</t>
+  </si>
+  <si>
+    <t>Verify Email</t>
+  </si>
+  <si>
+    <t>Email should be in a format like
+(eg. name@domain.com)</t>
+  </si>
+  <si>
+    <t>A.012</t>
+  </si>
+  <si>
+    <t>A.013</t>
+  </si>
+  <si>
+    <t>Valid Name, Phone, and Mail (domain missing)</t>
+  </si>
+  <si>
+    <t>Valid Name, Phone, and Mail (wrong domain format)</t>
+  </si>
+  <si>
+    <t>A.014</t>
+  </si>
+  <si>
+    <t>A.015</t>
+  </si>
+  <si>
+    <t>Valid Name, Phone, and Mail (with Multiple '@' Characters)</t>
+  </si>
+  <si>
+    <t>Valid Name, Phone, and Mail (with Missing '@' Character)</t>
+  </si>
+  <si>
+    <t>Valid Name, Phone, and Mail
+(has a 254 char)</t>
+  </si>
+  <si>
+    <t>Valid Name, Phone, and Mail
+(has a 255 char)</t>
+  </si>
+  <si>
+    <t>Mail MAX LENGTH is 254</t>
+  </si>
+  <si>
+    <t>Mail cannot be repeated</t>
+  </si>
+  <si>
+    <t>Valid Name, Phone, and Mail. and then add a valid Name, Valid Phone num, and repeat the same  Mail</t>
+  </si>
+  <si>
+    <t>A.016</t>
+  </si>
+  <si>
+    <t>A.017</t>
+  </si>
+  <si>
+    <t>A.018</t>
+  </si>
+  <si>
+    <t>A.019</t>
+  </si>
+  <si>
+    <t>U.001</t>
+  </si>
+  <si>
+    <t>Verify Update a Phone Number</t>
+  </si>
+  <si>
+    <t>Update Phone Number</t>
+  </si>
+  <si>
+    <t>U.002</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, Phone, and Mail</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, Phone num has a char or special char, and Valid Mail</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, 11 digits for Phone num starting with (01), and Valid Mail</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, 12 digits for Phone num starting with (01), and Valid Mail</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, 11 digits for Phone num and doesn't start with (01), and Valid Mail</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, Repeated Phone num, and another Valid Mail</t>
+  </si>
+  <si>
+    <t>U.003</t>
+  </si>
+  <si>
+    <t>U.004</t>
+  </si>
+  <si>
+    <t>U.005</t>
+  </si>
+  <si>
+    <t>U.006</t>
+  </si>
+  <si>
+    <t>U.007</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using 255 char for Name. and a Valid Phone, and Mail</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using 256 char for Name. and a Valid Phone, and Mail</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using an inValid Name. and a Valid Phone, and Mail</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Repeated Name, Valid Phone num, and another Valid Mail</t>
+  </si>
+  <si>
+    <t>U.008</t>
+  </si>
+  <si>
+    <t>U.009</t>
+  </si>
+  <si>
+    <t>U.010</t>
+  </si>
+  <si>
+    <t>U.011</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, Phone, and Mail (domain missing)</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, Phone, and Mail (wrong domain format)</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, Phone, and Mail (with Multiple '@' Characters)</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, Phone, and Mail (with Missing '@' Character)</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, Phone, and Mail
+(has a 254 char)</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, Phone, and Mail
+(has a 255 char)</t>
+  </si>
+  <si>
+    <t>Update the Phone Number, Name, and Mail,
+Using a Valid Name, Phone Num, and  repeated  Mail</t>
+  </si>
+  <si>
+    <t>U.012</t>
+  </si>
+  <si>
+    <t>U.013</t>
+  </si>
+  <si>
+    <t>U.014</t>
+  </si>
+  <si>
+    <t>U.015</t>
+  </si>
+  <si>
+    <t>U.016</t>
+  </si>
+  <si>
+    <t>U.017</t>
+  </si>
+  <si>
+    <t>Delete a phone number</t>
+  </si>
+  <si>
+    <t>Add a Valid Phone Number, Valid Name, and Valid Name.
+and then try to delete that contact using the right Phone number</t>
+  </si>
+  <si>
+    <t>Verify Delete a phone number</t>
+  </si>
+  <si>
+    <t>Add a Valid Phone Number, Valid Name, and Valid Name.
+and then try to delete that contact using the wrong phone number with one digit wrong.</t>
+  </si>
+  <si>
+    <t>Add a Valid Phone Number, Valid Name, and Valid Name.
+and then try to delete that contact using the wrong Phone number that has the wrong beginning (eg. 11 instead of 01 )</t>
+  </si>
+  <si>
+    <t>Try to delete a Valid Phone number that does not exist ( never added before)</t>
+  </si>
+  <si>
+    <t>D.001</t>
+  </si>
+  <si>
+    <t>D.002</t>
+  </si>
+  <si>
+    <t>D.003</t>
+  </si>
+  <si>
+    <t>D.004</t>
   </si>
 </sst>
 </file>
@@ -583,7 +809,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,6 +858,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -660,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -758,6 +1008,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1078,11 +1364,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J108"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" customHeight="1"/>
@@ -1482,77 +1768,1736 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" ht="13">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" ht="12.5">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" ht="12.5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" ht="12.5">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" ht="13">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="8"/>
+    <row r="13" spans="1:10" s="38" customFormat="1" ht="55" customHeight="1">
+      <c r="A13" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="38" customFormat="1" ht="55" customHeight="1">
+      <c r="A14" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37"/>
+    </row>
+    <row r="15" spans="1:10" s="38" customFormat="1" ht="55" customHeight="1">
+      <c r="A15" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="37"/>
+    </row>
+    <row r="16" spans="1:10" s="38" customFormat="1" ht="55" customHeight="1">
+      <c r="A16" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="37"/>
+    </row>
+    <row r="17" spans="1:10" s="38" customFormat="1" ht="55" customHeight="1">
+      <c r="A17" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
+    </row>
+    <row r="18" spans="1:10" s="38" customFormat="1" ht="55" customHeight="1">
+      <c r="A18" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="1:10" s="38" customFormat="1" ht="55" customHeight="1">
+      <c r="A19" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="37"/>
+    </row>
+    <row r="20" spans="1:10" s="38" customFormat="1" ht="55" customHeight="1">
+      <c r="A20" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="37"/>
+    </row>
+    <row r="21" spans="1:10" ht="13">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="13">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="12.5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" ht="12.5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="12.5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" ht="13">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="12.5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" ht="12.5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="12.5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" ht="13">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" ht="12.5">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" ht="12.5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" ht="12.5">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" ht="12.5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" ht="13">
+      <c r="A35" s="1"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" ht="13">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="8"/>
+    </row>
+    <row r="37" spans="1:10" ht="12.5">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" ht="13">
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" ht="13">
+      <c r="A39" s="1"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" ht="12.5">
+      <c r="A40" s="1"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:10" ht="12.5">
+      <c r="A41" s="1"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" ht="12.5">
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="1:10" ht="13">
+      <c r="A43" s="1"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="8"/>
+    </row>
+    <row r="44" spans="1:10" ht="13">
+      <c r="A44" s="9"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="8"/>
+    </row>
+    <row r="45" spans="1:10" ht="12.5">
+      <c r="A45" s="9"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="11"/>
+    </row>
+    <row r="46" spans="1:10" ht="12.5">
+      <c r="A46" s="9"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="11"/>
+    </row>
+    <row r="47" spans="1:10" ht="12.5">
+      <c r="A47" s="9"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="1:10" ht="12.5">
+      <c r="A48" s="9"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="11"/>
+    </row>
+    <row r="49" spans="1:10" ht="12.5">
+      <c r="A49" s="12"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="14"/>
+    </row>
+    <row r="50" spans="1:10" ht="12.5">
+      <c r="A50" s="12"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="14"/>
+    </row>
+    <row r="51" spans="1:10" ht="12.5">
+      <c r="A51" s="12"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="14"/>
+    </row>
+    <row r="52" spans="1:10" ht="12.5">
+      <c r="A52" s="12"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="14"/>
+    </row>
+    <row r="53" spans="1:10" ht="12.5">
+      <c r="A53" s="12"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="14"/>
+    </row>
+    <row r="54" spans="1:10" ht="12.5">
+      <c r="A54" s="12"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="14"/>
+    </row>
+    <row r="55" spans="1:10" ht="12.5">
+      <c r="A55" s="12"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="14"/>
+    </row>
+    <row r="56" spans="1:10" ht="12.5">
+      <c r="A56" s="12"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="1:10" ht="12.5">
+      <c r="A57" s="12"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="1:10" ht="12.5">
+      <c r="A58" s="12"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="14"/>
+    </row>
+    <row r="59" spans="1:10" ht="12.5">
+      <c r="A59" s="12"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="14"/>
+    </row>
+    <row r="60" spans="1:10" ht="12.5">
+      <c r="A60" s="12"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="14"/>
+    </row>
+    <row r="61" spans="1:10" ht="12.5">
+      <c r="A61" s="12"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="14"/>
+    </row>
+    <row r="62" spans="1:10" ht="12.5">
+      <c r="A62" s="12"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="14"/>
+    </row>
+    <row r="63" spans="1:10" ht="12.5">
+      <c r="A63" s="12"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="14"/>
+    </row>
+    <row r="64" spans="1:10" ht="12.5">
+      <c r="A64" s="12"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="14"/>
+    </row>
+    <row r="65" spans="1:10" ht="12.5">
+      <c r="A65" s="12"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="14"/>
+    </row>
+    <row r="66" spans="1:10" ht="12.5">
+      <c r="A66" s="12"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="14"/>
+    </row>
+    <row r="67" spans="1:10" ht="12.5">
+      <c r="A67" s="12"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="14"/>
+    </row>
+    <row r="68" spans="1:10" ht="12.5">
+      <c r="A68" s="12"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="14"/>
+    </row>
+    <row r="69" spans="1:10" ht="12.5">
+      <c r="A69" s="12"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="14"/>
+    </row>
+    <row r="70" spans="1:10" ht="12.5">
+      <c r="A70" s="12"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="14"/>
+    </row>
+    <row r="71" spans="1:10" ht="12.5">
+      <c r="A71" s="12"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="14"/>
+    </row>
+    <row r="72" spans="1:10" ht="12.5">
+      <c r="A72" s="12"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="14"/>
+    </row>
+    <row r="73" spans="1:10" ht="12.5">
+      <c r="A73" s="12"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="14"/>
+    </row>
+    <row r="74" spans="1:10" ht="12.5">
+      <c r="A74" s="12"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="14"/>
+    </row>
+    <row r="75" spans="1:10" ht="12.5">
+      <c r="A75" s="12"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="14"/>
+    </row>
+    <row r="76" spans="1:10" ht="12.5">
+      <c r="A76" s="12"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="14"/>
+    </row>
+    <row r="77" spans="1:10" ht="12.5">
+      <c r="A77" s="12"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="14"/>
+    </row>
+    <row r="78" spans="1:10" ht="12.5">
+      <c r="A78" s="12"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="14"/>
+    </row>
+    <row r="79" spans="1:10" ht="12.5">
+      <c r="A79" s="12"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="14"/>
+    </row>
+    <row r="80" spans="1:10" ht="12.5">
+      <c r="A80" s="12"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="14"/>
+    </row>
+    <row r="81" spans="1:10" ht="12.5">
+      <c r="A81" s="12"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="14"/>
+    </row>
+    <row r="82" spans="1:10" ht="12.5">
+      <c r="A82" s="12"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="14"/>
+    </row>
+    <row r="83" spans="1:10" ht="12.5">
+      <c r="A83" s="12"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="14"/>
+    </row>
+    <row r="84" spans="1:10" ht="12.5">
+      <c r="A84" s="12"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="14"/>
+    </row>
+    <row r="85" spans="1:10" ht="12.5">
+      <c r="A85" s="12"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="14"/>
+    </row>
+    <row r="86" spans="1:10" ht="12.5">
+      <c r="A86" s="12"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="12"/>
+      <c r="J86" s="14"/>
+    </row>
+    <row r="87" spans="1:10" ht="12.5">
+      <c r="A87" s="12"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="12"/>
+      <c r="J87" s="14"/>
+    </row>
+    <row r="88" spans="1:10" ht="12.5">
+      <c r="A88" s="12"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="12"/>
+      <c r="J88" s="14"/>
+    </row>
+    <row r="89" spans="1:10" ht="12.5">
+      <c r="A89" s="12"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="12"/>
+      <c r="J89" s="14"/>
+    </row>
+    <row r="90" spans="1:10" ht="12.5">
+      <c r="A90" s="12"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="12"/>
+      <c r="J90" s="14"/>
+    </row>
+    <row r="91" spans="1:10" ht="12.5">
+      <c r="A91" s="12"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="12"/>
+      <c r="J91" s="14"/>
+    </row>
+    <row r="92" spans="1:10" ht="12.5">
+      <c r="A92" s="12"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="12"/>
+      <c r="J92" s="14"/>
+    </row>
+    <row r="93" spans="1:10" ht="12.5">
+      <c r="A93" s="12"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="12"/>
+      <c r="J93" s="14"/>
+    </row>
+    <row r="94" spans="1:10" ht="12.5">
+      <c r="A94" s="12"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="12"/>
+      <c r="J94" s="14"/>
+    </row>
+    <row r="95" spans="1:10" ht="12.5">
+      <c r="A95" s="12"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="14"/>
+    </row>
+    <row r="96" spans="1:10" ht="12.5">
+      <c r="A96" s="12"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="12"/>
+      <c r="J96" s="14"/>
+    </row>
+    <row r="97" spans="1:10" ht="12.5">
+      <c r="A97" s="12"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="14"/>
+    </row>
+    <row r="98" spans="1:10" ht="12.5">
+      <c r="A98" s="12"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="12"/>
+      <c r="J98" s="14"/>
+    </row>
+    <row r="99" spans="1:10" ht="12.5">
+      <c r="A99" s="12"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="12"/>
+      <c r="J99" s="14"/>
+    </row>
+    <row r="100" spans="1:10" ht="12.5">
+      <c r="A100" s="12"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="12"/>
+      <c r="J100" s="14"/>
+    </row>
+    <row r="101" spans="1:10" ht="12.5">
+      <c r="A101" s="12"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="12"/>
+      <c r="J101" s="14"/>
+    </row>
+    <row r="102" spans="1:10" ht="12.5">
+      <c r="A102" s="12"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="13"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="12"/>
+      <c r="J102" s="14"/>
+    </row>
+    <row r="103" spans="1:10" ht="12.5">
+      <c r="A103" s="12"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="13"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="12"/>
+      <c r="J103" s="14"/>
+    </row>
+    <row r="104" spans="1:10" ht="12.5">
+      <c r="A104" s="12"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="13"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="12"/>
+      <c r="J104" s="14"/>
+    </row>
+    <row r="105" spans="1:10" ht="12.5">
+      <c r="A105" s="12"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="12"/>
+      <c r="J105" s="14"/>
+    </row>
+    <row r="106" spans="1:10" ht="12.5">
+      <c r="A106" s="12"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="13"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="12"/>
+      <c r="J106" s="14"/>
+    </row>
+    <row r="107" spans="1:10" ht="12.5">
+      <c r="A107" s="12"/>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="12"/>
+      <c r="J107" s="14"/>
+    </row>
+    <row r="108" spans="1:10" ht="12.5">
+      <c r="A108" s="12"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="12"/>
+      <c r="J108" s="14"/>
+    </row>
+    <row r="109" spans="1:10" ht="12.5">
+      <c r="A109" s="12"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="13"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="12"/>
+      <c r="J109" s="14"/>
+    </row>
+    <row r="110" spans="1:10" ht="12.5">
+      <c r="A110" s="12"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="13"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="12"/>
+      <c r="J110" s="14"/>
+    </row>
+    <row r="111" spans="1:10" ht="12.5">
+      <c r="A111" s="12"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="12"/>
+      <c r="J111" s="14"/>
+    </row>
+    <row r="112" spans="1:10" ht="12.5">
+      <c r="A112" s="12"/>
+      <c r="B112" s="6"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="12"/>
+      <c r="J112" s="14"/>
+    </row>
+    <row r="113" spans="1:10" ht="12.5">
+      <c r="A113" s="12"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="13"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="12"/>
+      <c r="J113" s="14"/>
+    </row>
+    <row r="114" spans="1:10" ht="12.5">
+      <c r="A114" s="12"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="13"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="12"/>
+      <c r="J114" s="14"/>
+    </row>
+    <row r="115" spans="1:10" ht="12.5">
+      <c r="A115" s="12"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="13"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="12"/>
+      <c r="J115" s="14"/>
+    </row>
+    <row r="116" spans="1:10" ht="12.5">
+      <c r="A116" s="12"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="13"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="12"/>
+      <c r="J116" s="14"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J116" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="3" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AD4FA8-926B-4E17-8CD6-03BD272653FB}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J98"/>
+  <sheetViews>
+    <sheetView zoomScale="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" customWidth="1"/>
+    <col min="4" max="4" width="33.26953125" customWidth="1"/>
+    <col min="5" max="5" width="39.08984375" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="26.08984375" customWidth="1"/>
+    <col min="8" max="8" width="28.26953125" customWidth="1"/>
+    <col min="9" max="10" width="15.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="32" customFormat="1" ht="55" customHeight="1">
+      <c r="A2" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:10" s="32" customFormat="1" ht="55" customHeight="1">
+      <c r="A3" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="1:10" s="32" customFormat="1" ht="55" customHeight="1">
+      <c r="A4" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:10" s="32" customFormat="1" ht="55" customHeight="1">
+      <c r="A5" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" s="32" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A6" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="31"/>
+    </row>
+    <row r="7" spans="1:10" s="32" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A7" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="31"/>
+    </row>
+    <row r="8" spans="1:10" s="44" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A8" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
+    </row>
+    <row r="9" spans="1:10" s="44" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A9" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="43"/>
+    </row>
+    <row r="10" spans="1:10" s="44" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A10" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="43"/>
+    </row>
+    <row r="11" spans="1:10" s="44" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A11" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" s="38" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A12" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="37"/>
+    </row>
+    <row r="13" spans="1:10" s="38" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A13" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="37"/>
+    </row>
+    <row r="14" spans="1:10" s="38" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A14" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37"/>
+    </row>
+    <row r="15" spans="1:10" s="38" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A15" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="37"/>
+    </row>
+    <row r="16" spans="1:10" s="38" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A16" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="37"/>
+    </row>
+    <row r="17" spans="1:10" s="38" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A17" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
+    </row>
+    <row r="18" spans="1:10" s="38" customFormat="1" ht="65.5" customHeight="1">
+      <c r="A18" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="37"/>
     </row>
     <row r="19" spans="1:10" ht="12.5">
       <c r="A19" s="1"/>
@@ -1566,7 +3511,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" ht="12.5">
+    <row r="20" spans="1:10" ht="13">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1575,10 +3520,10 @@
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" ht="12.5">
+      <c r="I20" s="7"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="13">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1587,10 +3532,10 @@
       <c r="F21" s="2"/>
       <c r="G21" s="3"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" ht="13">
+      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="12.5">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1599,8 +3544,8 @@
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="8"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" ht="12.5">
       <c r="A23" s="1"/>
@@ -1626,197 +3571,197 @@
       <c r="I24" s="1"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" ht="12.5">
+    <row r="25" spans="1:10" ht="13">
       <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" ht="12.5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" ht="13">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:10" ht="13">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="8"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="13">
+      <c r="A26" s="9"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="12.5">
+      <c r="A27" s="9"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:10" ht="12.5">
+      <c r="A28" s="9"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" ht="12.5">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" ht="13">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="8"/>
-    </row>
-    <row r="31" spans="1:10" ht="13">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="8"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="1:10" ht="12.5">
+      <c r="A30" s="9"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="1:10" ht="12.5">
+      <c r="A31" s="12"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="14"/>
     </row>
     <row r="32" spans="1:10" ht="12.5">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="4"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="14"/>
     </row>
     <row r="33" spans="1:10" ht="12.5">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="4"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="14"/>
     </row>
     <row r="34" spans="1:10" ht="12.5">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10" ht="13">
-      <c r="A35" s="1"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" spans="1:10" ht="13">
-      <c r="A36" s="9"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="8"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="14"/>
+    </row>
+    <row r="35" spans="1:10" ht="12.5">
+      <c r="A35" s="12"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="1:10" ht="12.5">
+      <c r="A36" s="12"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="14"/>
     </row>
     <row r="37" spans="1:10" ht="12.5">
-      <c r="A37" s="9"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="11"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="14"/>
     </row>
     <row r="38" spans="1:10" ht="12.5">
-      <c r="A38" s="9"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="11"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="14"/>
     </row>
     <row r="39" spans="1:10" ht="12.5">
-      <c r="A39" s="9"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="11"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="14"/>
     </row>
     <row r="40" spans="1:10" ht="12.5">
-      <c r="A40" s="9"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="11"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="14"/>
     </row>
     <row r="41" spans="1:10" ht="12.5">
       <c r="A41" s="12"/>
@@ -2514,128 +4459,8 @@
       <c r="I98" s="12"/>
       <c r="J98" s="14"/>
     </row>
-    <row r="99" spans="1:10" ht="12.5">
-      <c r="A99" s="12"/>
-      <c r="B99" s="6"/>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="6"/>
-      <c r="F99" s="6"/>
-      <c r="G99" s="13"/>
-      <c r="H99" s="6"/>
-      <c r="I99" s="12"/>
-      <c r="J99" s="14"/>
-    </row>
-    <row r="100" spans="1:10" ht="12.5">
-      <c r="A100" s="12"/>
-      <c r="B100" s="6"/>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="6"/>
-      <c r="F100" s="6"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="6"/>
-      <c r="I100" s="12"/>
-      <c r="J100" s="14"/>
-    </row>
-    <row r="101" spans="1:10" ht="12.5">
-      <c r="A101" s="12"/>
-      <c r="B101" s="6"/>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="6"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="6"/>
-      <c r="I101" s="12"/>
-      <c r="J101" s="14"/>
-    </row>
-    <row r="102" spans="1:10" ht="12.5">
-      <c r="A102" s="12"/>
-      <c r="B102" s="6"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6"/>
-      <c r="F102" s="6"/>
-      <c r="G102" s="13"/>
-      <c r="H102" s="6"/>
-      <c r="I102" s="12"/>
-      <c r="J102" s="14"/>
-    </row>
-    <row r="103" spans="1:10" ht="12.5">
-      <c r="A103" s="12"/>
-      <c r="B103" s="6"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="13"/>
-      <c r="H103" s="6"/>
-      <c r="I103" s="12"/>
-      <c r="J103" s="14"/>
-    </row>
-    <row r="104" spans="1:10" ht="12.5">
-      <c r="A104" s="12"/>
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="13"/>
-      <c r="H104" s="6"/>
-      <c r="I104" s="12"/>
-      <c r="J104" s="14"/>
-    </row>
-    <row r="105" spans="1:10" ht="12.5">
-      <c r="A105" s="12"/>
-      <c r="B105" s="6"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="13"/>
-      <c r="H105" s="6"/>
-      <c r="I105" s="12"/>
-      <c r="J105" s="14"/>
-    </row>
-    <row r="106" spans="1:10" ht="12.5">
-      <c r="A106" s="12"/>
-      <c r="B106" s="6"/>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="6"/>
-      <c r="F106" s="6"/>
-      <c r="G106" s="13"/>
-      <c r="H106" s="6"/>
-      <c r="I106" s="12"/>
-      <c r="J106" s="14"/>
-    </row>
-    <row r="107" spans="1:10" ht="12.5">
-      <c r="A107" s="12"/>
-      <c r="B107" s="6"/>
-      <c r="C107" s="6"/>
-      <c r="D107" s="6"/>
-      <c r="E107" s="6"/>
-      <c r="F107" s="6"/>
-      <c r="G107" s="13"/>
-      <c r="H107" s="6"/>
-      <c r="I107" s="12"/>
-      <c r="J107" s="14"/>
-    </row>
-    <row r="108" spans="1:10" ht="12.5">
-      <c r="A108" s="12"/>
-      <c r="B108" s="6"/>
-      <c r="C108" s="6"/>
-      <c r="D108" s="6"/>
-      <c r="E108" s="6"/>
-      <c r="F108" s="6"/>
-      <c r="G108" s="13"/>
-      <c r="H108" s="6"/>
-      <c r="I108" s="12"/>
-      <c r="J108" s="14"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J108" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:J98" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -2643,7 +4468,2196 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A6D626-9CA0-4ED4-8484-F81D89F65226}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J84"/>
+  <sheetViews>
+    <sheetView zoomScale="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" customWidth="1"/>
+    <col min="4" max="4" width="33.26953125" customWidth="1"/>
+    <col min="5" max="5" width="39.08984375" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="26.08984375" customWidth="1"/>
+    <col min="8" max="8" width="28.26953125" customWidth="1"/>
+    <col min="9" max="10" width="15.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="32" customFormat="1" ht="55" customHeight="1">
+      <c r="A2" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:10" s="32" customFormat="1" ht="79" customHeight="1">
+      <c r="A3" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="1:10" s="32" customFormat="1" ht="71.5" customHeight="1">
+      <c r="A4" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:10" s="32" customFormat="1" ht="71.5" customHeight="1">
+      <c r="A5" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" ht="13">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="13">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="12.5">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="12.5">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="12.5">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="13">
+      <c r="A11" s="1"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="13">
+      <c r="A12" s="9"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="12.5">
+      <c r="A13" s="9"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" ht="12.5">
+      <c r="A14" s="9"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" ht="12.5">
+      <c r="A15" s="9"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" ht="12.5">
+      <c r="A16" s="9"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" ht="12.5">
+      <c r="A17" s="12"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" ht="12.5">
+      <c r="A18" s="12"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" ht="12.5">
+      <c r="A19" s="12"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="1:10" ht="12.5">
+      <c r="A20" s="12"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.5">
+      <c r="A21" s="12"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:10" ht="12.5">
+      <c r="A22" s="12"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="1:10" ht="12.5">
+      <c r="A23" s="12"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="1:10" ht="12.5">
+      <c r="A24" s="12"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:10" ht="12.5">
+      <c r="A25" s="12"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="1:10" ht="12.5">
+      <c r="A26" s="12"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:10" ht="12.5">
+      <c r="A27" s="12"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="1:10" ht="12.5">
+      <c r="A28" s="12"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="1:10" ht="12.5">
+      <c r="A29" s="12"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" ht="12.5">
+      <c r="A30" s="12"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="1:10" ht="12.5">
+      <c r="A31" s="12"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="1:10" ht="12.5">
+      <c r="A32" s="12"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="1:10" ht="12.5">
+      <c r="A33" s="12"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="1:10" ht="12.5">
+      <c r="A34" s="12"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="14"/>
+    </row>
+    <row r="35" spans="1:10" ht="12.5">
+      <c r="A35" s="12"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="1:10" ht="12.5">
+      <c r="A36" s="12"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="1:10" ht="12.5">
+      <c r="A37" s="12"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="14"/>
+    </row>
+    <row r="38" spans="1:10" ht="12.5">
+      <c r="A38" s="12"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" spans="1:10" ht="12.5">
+      <c r="A39" s="12"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="14"/>
+    </row>
+    <row r="40" spans="1:10" ht="12.5">
+      <c r="A40" s="12"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="14"/>
+    </row>
+    <row r="41" spans="1:10" ht="12.5">
+      <c r="A41" s="12"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="1:10" ht="12.5">
+      <c r="A42" s="12"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="1:10" ht="12.5">
+      <c r="A43" s="12"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="14"/>
+    </row>
+    <row r="44" spans="1:10" ht="12.5">
+      <c r="A44" s="12"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="14"/>
+    </row>
+    <row r="45" spans="1:10" ht="12.5">
+      <c r="A45" s="12"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="14"/>
+    </row>
+    <row r="46" spans="1:10" ht="12.5">
+      <c r="A46" s="12"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="14"/>
+    </row>
+    <row r="47" spans="1:10" ht="12.5">
+      <c r="A47" s="12"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="1:10" ht="12.5">
+      <c r="A48" s="12"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="14"/>
+    </row>
+    <row r="49" spans="1:10" ht="12.5">
+      <c r="A49" s="12"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="14"/>
+    </row>
+    <row r="50" spans="1:10" ht="12.5">
+      <c r="A50" s="12"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="14"/>
+    </row>
+    <row r="51" spans="1:10" ht="12.5">
+      <c r="A51" s="12"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="14"/>
+    </row>
+    <row r="52" spans="1:10" ht="12.5">
+      <c r="A52" s="12"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="14"/>
+    </row>
+    <row r="53" spans="1:10" ht="12.5">
+      <c r="A53" s="12"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="14"/>
+    </row>
+    <row r="54" spans="1:10" ht="12.5">
+      <c r="A54" s="12"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="14"/>
+    </row>
+    <row r="55" spans="1:10" ht="12.5">
+      <c r="A55" s="12"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="14"/>
+    </row>
+    <row r="56" spans="1:10" ht="12.5">
+      <c r="A56" s="12"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="1:10" ht="12.5">
+      <c r="A57" s="12"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="1:10" ht="12.5">
+      <c r="A58" s="12"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="14"/>
+    </row>
+    <row r="59" spans="1:10" ht="12.5">
+      <c r="A59" s="12"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="14"/>
+    </row>
+    <row r="60" spans="1:10" ht="12.5">
+      <c r="A60" s="12"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="14"/>
+    </row>
+    <row r="61" spans="1:10" ht="12.5">
+      <c r="A61" s="12"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="14"/>
+    </row>
+    <row r="62" spans="1:10" ht="12.5">
+      <c r="A62" s="12"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="14"/>
+    </row>
+    <row r="63" spans="1:10" ht="12.5">
+      <c r="A63" s="12"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="14"/>
+    </row>
+    <row r="64" spans="1:10" ht="12.5">
+      <c r="A64" s="12"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="14"/>
+    </row>
+    <row r="65" spans="1:10" ht="12.5">
+      <c r="A65" s="12"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="14"/>
+    </row>
+    <row r="66" spans="1:10" ht="12.5">
+      <c r="A66" s="12"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="14"/>
+    </row>
+    <row r="67" spans="1:10" ht="12.5">
+      <c r="A67" s="12"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="14"/>
+    </row>
+    <row r="68" spans="1:10" ht="12.5">
+      <c r="A68" s="12"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="14"/>
+    </row>
+    <row r="69" spans="1:10" ht="12.5">
+      <c r="A69" s="12"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="14"/>
+    </row>
+    <row r="70" spans="1:10" ht="12.5">
+      <c r="A70" s="12"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="14"/>
+    </row>
+    <row r="71" spans="1:10" ht="12.5">
+      <c r="A71" s="12"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="14"/>
+    </row>
+    <row r="72" spans="1:10" ht="12.5">
+      <c r="A72" s="12"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="14"/>
+    </row>
+    <row r="73" spans="1:10" ht="12.5">
+      <c r="A73" s="12"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="14"/>
+    </row>
+    <row r="74" spans="1:10" ht="12.5">
+      <c r="A74" s="12"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="14"/>
+    </row>
+    <row r="75" spans="1:10" ht="12.5">
+      <c r="A75" s="12"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="14"/>
+    </row>
+    <row r="76" spans="1:10" ht="12.5">
+      <c r="A76" s="12"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="14"/>
+    </row>
+    <row r="77" spans="1:10" ht="12.5">
+      <c r="A77" s="12"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="14"/>
+    </row>
+    <row r="78" spans="1:10" ht="12.5">
+      <c r="A78" s="12"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="14"/>
+    </row>
+    <row r="79" spans="1:10" ht="12.5">
+      <c r="A79" s="12"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="14"/>
+    </row>
+    <row r="80" spans="1:10" ht="12.5">
+      <c r="A80" s="12"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="14"/>
+    </row>
+    <row r="81" spans="1:10" ht="12.5">
+      <c r="A81" s="12"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="14"/>
+    </row>
+    <row r="82" spans="1:10" ht="12.5">
+      <c r="A82" s="12"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="14"/>
+    </row>
+    <row r="83" spans="1:10" ht="12.5">
+      <c r="A83" s="12"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="14"/>
+    </row>
+    <row r="84" spans="1:10" ht="12.5">
+      <c r="A84" s="12"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="14"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J84" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="3" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA28810-EE9E-4120-9C69-BC37614E8ABB}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" customWidth="1"/>
+    <col min="4" max="4" width="33.26953125" customWidth="1"/>
+    <col min="5" max="5" width="39.08984375" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="26.08984375" customWidth="1"/>
+    <col min="8" max="8" width="28.26953125" customWidth="1"/>
+    <col min="9" max="10" width="15.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="32" customFormat="1" ht="55" customHeight="1">
+      <c r="A2" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:10" s="32" customFormat="1" ht="79" customHeight="1">
+      <c r="A3" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="1:10" s="32" customFormat="1" ht="71.5" customHeight="1">
+      <c r="A4" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:10" s="32" customFormat="1" ht="71.5" customHeight="1">
+      <c r="A5" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" ht="13">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="13">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="12.5">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="12.5">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="12.5">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="13">
+      <c r="A11" s="1"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="13">
+      <c r="A12" s="9"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="12.5">
+      <c r="A13" s="9"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" ht="12.5">
+      <c r="A14" s="9"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" ht="12.5">
+      <c r="A15" s="9"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" ht="12.5">
+      <c r="A16" s="9"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" ht="12.5">
+      <c r="A17" s="12"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" ht="12.5">
+      <c r="A18" s="12"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" ht="12.5">
+      <c r="A19" s="12"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="1:10" ht="12.5">
+      <c r="A20" s="12"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.5">
+      <c r="A21" s="12"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:10" ht="12.5">
+      <c r="A22" s="12"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="1:10" ht="12.5">
+      <c r="A23" s="12"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="1:10" ht="12.5">
+      <c r="A24" s="12"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:10" ht="12.5">
+      <c r="A25" s="12"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="1:10" ht="12.5">
+      <c r="A26" s="12"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:10" ht="12.5">
+      <c r="A27" s="12"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="1:10" ht="12.5">
+      <c r="A28" s="12"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="1:10" ht="12.5">
+      <c r="A29" s="12"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" ht="12.5">
+      <c r="A30" s="12"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="1:10" ht="12.5">
+      <c r="A31" s="12"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="1:10" ht="12.5">
+      <c r="A32" s="12"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="1:10" ht="12.5">
+      <c r="A33" s="12"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="1:10" ht="12.5">
+      <c r="A34" s="12"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="14"/>
+    </row>
+    <row r="35" spans="1:10" ht="12.5">
+      <c r="A35" s="12"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="1:10" ht="12.5">
+      <c r="A36" s="12"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="1:10" ht="12.5">
+      <c r="A37" s="12"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="14"/>
+    </row>
+    <row r="38" spans="1:10" ht="12.5">
+      <c r="A38" s="12"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" spans="1:10" ht="12.5">
+      <c r="A39" s="12"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="14"/>
+    </row>
+    <row r="40" spans="1:10" ht="12.5">
+      <c r="A40" s="12"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="14"/>
+    </row>
+    <row r="41" spans="1:10" ht="12.5">
+      <c r="A41" s="12"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="1:10" ht="12.5">
+      <c r="A42" s="12"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="1:10" ht="12.5">
+      <c r="A43" s="12"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="14"/>
+    </row>
+    <row r="44" spans="1:10" ht="12.5">
+      <c r="A44" s="12"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="14"/>
+    </row>
+    <row r="45" spans="1:10" ht="12.5">
+      <c r="A45" s="12"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="14"/>
+    </row>
+    <row r="46" spans="1:10" ht="12.5">
+      <c r="A46" s="12"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="14"/>
+    </row>
+    <row r="47" spans="1:10" ht="12.5">
+      <c r="A47" s="12"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="1:10" ht="12.5">
+      <c r="A48" s="12"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="14"/>
+    </row>
+    <row r="49" spans="1:10" ht="12.5">
+      <c r="A49" s="12"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="14"/>
+    </row>
+    <row r="50" spans="1:10" ht="12.5">
+      <c r="A50" s="12"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="14"/>
+    </row>
+    <row r="51" spans="1:10" ht="12.5">
+      <c r="A51" s="12"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="14"/>
+    </row>
+    <row r="52" spans="1:10" ht="12.5">
+      <c r="A52" s="12"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="14"/>
+    </row>
+    <row r="53" spans="1:10" ht="12.5">
+      <c r="A53" s="12"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="14"/>
+    </row>
+    <row r="54" spans="1:10" ht="12.5">
+      <c r="A54" s="12"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="14"/>
+    </row>
+    <row r="55" spans="1:10" ht="12.5">
+      <c r="A55" s="12"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="14"/>
+    </row>
+    <row r="56" spans="1:10" ht="12.5">
+      <c r="A56" s="12"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="1:10" ht="12.5">
+      <c r="A57" s="12"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="1:10" ht="12.5">
+      <c r="A58" s="12"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="14"/>
+    </row>
+    <row r="59" spans="1:10" ht="12.5">
+      <c r="A59" s="12"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="14"/>
+    </row>
+    <row r="60" spans="1:10" ht="12.5">
+      <c r="A60" s="12"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="14"/>
+    </row>
+    <row r="61" spans="1:10" ht="12.5">
+      <c r="A61" s="12"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="14"/>
+    </row>
+    <row r="62" spans="1:10" ht="12.5">
+      <c r="A62" s="12"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="14"/>
+    </row>
+    <row r="63" spans="1:10" ht="12.5">
+      <c r="A63" s="12"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="14"/>
+    </row>
+    <row r="64" spans="1:10" ht="12.5">
+      <c r="A64" s="12"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="14"/>
+    </row>
+    <row r="65" spans="1:10" ht="12.5">
+      <c r="A65" s="12"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="14"/>
+    </row>
+    <row r="66" spans="1:10" ht="12.5">
+      <c r="A66" s="12"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="14"/>
+    </row>
+    <row r="67" spans="1:10" ht="12.5">
+      <c r="A67" s="12"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="14"/>
+    </row>
+    <row r="68" spans="1:10" ht="12.5">
+      <c r="A68" s="12"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="14"/>
+    </row>
+    <row r="69" spans="1:10" ht="12.5">
+      <c r="A69" s="12"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="14"/>
+    </row>
+    <row r="70" spans="1:10" ht="12.5">
+      <c r="A70" s="12"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="14"/>
+    </row>
+    <row r="71" spans="1:10" ht="12.5">
+      <c r="A71" s="12"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="14"/>
+    </row>
+    <row r="72" spans="1:10" ht="12.5">
+      <c r="A72" s="12"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="14"/>
+    </row>
+    <row r="73" spans="1:10" ht="12.5">
+      <c r="A73" s="12"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="14"/>
+    </row>
+    <row r="74" spans="1:10" ht="12.5">
+      <c r="A74" s="12"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="14"/>
+    </row>
+    <row r="75" spans="1:10" ht="12.5">
+      <c r="A75" s="12"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="14"/>
+    </row>
+    <row r="76" spans="1:10" ht="12.5">
+      <c r="A76" s="12"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="14"/>
+    </row>
+    <row r="77" spans="1:10" ht="12.5">
+      <c r="A77" s="12"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="14"/>
+    </row>
+    <row r="78" spans="1:10" ht="12.5">
+      <c r="A78" s="12"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="14"/>
+    </row>
+    <row r="79" spans="1:10" ht="12.5">
+      <c r="A79" s="12"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="14"/>
+    </row>
+    <row r="80" spans="1:10" ht="12.5">
+      <c r="A80" s="12"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="14"/>
+    </row>
+    <row r="81" spans="1:10" ht="12.5">
+      <c r="A81" s="12"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="14"/>
+    </row>
+    <row r="82" spans="1:10" ht="12.5">
+      <c r="A82" s="12"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="14"/>
+    </row>
+    <row r="83" spans="1:10" ht="12.5">
+      <c r="A83" s="12"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="14"/>
+    </row>
+    <row r="84" spans="1:10" ht="12.5">
+      <c r="A84" s="12"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="14"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J84" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="3" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2827,7 +6841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2921,7 +6935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3161,7 +7175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>